<commit_message>
Testrun2 and adjust metrics
</commit_message>
<xml_diff>
--- a/result/complex/complex1/LengthAngleSafety.xlsx
+++ b/result/complex/complex1/LengthAngleSafety.xlsx
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6945765349190751</v>
+        <v>0.6325197058534924</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02989882231648193</v>
+        <v>0.02765385105211411</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9592050554036922</v>
+        <v>0.8661309802792049</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DWA and update result
</commit_message>
<xml_diff>
--- a/result/complex/complex1/LengthAngleSafety.xlsx
+++ b/result/complex/complex1/LengthAngleSafety.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
         <v>0.0331819285339077</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001612903225806451</v>
+        <v>0.001082428676132903</v>
       </c>
       <c r="E2" t="n">
         <v>0.03793360398700971</v>
@@ -487,7 +487,7 @@
         <v>0.2225503592125709</v>
       </c>
       <c r="D3" t="n">
-        <v>0.009595535341943059</v>
+        <v>0.006346374577701655</v>
       </c>
       <c r="E3" t="n">
         <v>0.2821506637863836</v>
@@ -506,7 +506,7 @@
         <v>0.7582811847691517</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03339032389217423</v>
+        <v>0.02162982972700522</v>
       </c>
       <c r="E4" t="n">
         <v>0.9559655724401779</v>
@@ -525,10 +525,29 @@
         <v>0.6325197058534924</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02765385105211411</v>
+        <v>0.01781899850550332</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8661309802792049</v>
+        <v>0.8661309802792048</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>DWA</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.9418132611637343</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.03023739526088455</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.9438686045747178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>